<commit_message>
add participant to groupe
</commit_message>
<xml_diff>
--- a/tests/Feature/excel/test-notok.xlsx
+++ b/tests/Feature/excel/test-notok.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11213"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cindyleschaud/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cindyleschaud/Sites/localhost/shop/tests/Feature/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF32DD36-DA44-4C48-A91E-99EC2A004B82}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17600" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17600" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="150000"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -27,24 +28,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
-  <si>
-    <t>cindy.leschaud@gmail.com</t>
-  </si>
-  <si>
-    <t>cindy@designpond.ch</t>
-  </si>
-  <si>
-    <t>info@designpond.ch</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>emaild</t>
   </si>
+  <si>
+    <t>hello@yahoo.fr</t>
+  </si>
+  <si>
+    <t>droitformation.web@gmail.com</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -96,6 +94,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -363,40 +364,34 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
+      <c r="A3" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
-        <v>2</v>
-      </c>
+      <c r="A4" s="1"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A3" r:id="rId1"/>
-    <hyperlink ref="A4" r:id="rId2"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>